<commit_message>
Remove scheduler and test files; add SUMMA dynamic implementation with benchmarking
</commit_message>
<xml_diff>
--- a/summa_benchmark_results.xlsx
+++ b/summa_benchmark_results.xlsx
@@ -450,7 +450,7 @@
         <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2017223834991455</v>
+        <v>0.1688094139099121</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1000</v>
       </c>
       <c r="B3" t="n">
-        <v>0.08727145195007324</v>
+        <v>0.07811379432678223</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>1500</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1324887275695801</v>
+        <v>0.1165955066680908</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>2000</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2152059078216553</v>
+        <v>0.1820666790008545</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>2500</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3146018981933594</v>
+        <v>0.301706075668335</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>3000</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4917585849761963</v>
+        <v>0.4560689926147461</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>3500</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5974082946777344</v>
+        <v>0.5821278095245361</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>4000</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8593635559082031</v>
+        <v>0.8846116065979004</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>4500</v>
       </c>
       <c r="B10" t="n">
-        <v>1.231931924819946</v>
+        <v>1.153199911117554</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>5000</v>
       </c>
       <c r="B11" t="n">
-        <v>1.523181915283203</v>
+        <v>1.496581077575684</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>5500</v>
       </c>
       <c r="B12" t="n">
-        <v>1.97294545173645</v>
+        <v>1.982256174087524</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>6000</v>
       </c>
       <c r="B13" t="n">
-        <v>2.442967653274536</v>
+        <v>2.42500376701355</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>6500</v>
       </c>
       <c r="B14" t="n">
-        <v>3.071830987930298</v>
+        <v>3.049225330352783</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>7000</v>
       </c>
       <c r="B15" t="n">
-        <v>3.681252717971802</v>
+        <v>3.665996313095093</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>7500</v>
       </c>
       <c r="B16" t="n">
-        <v>4.424172401428223</v>
+        <v>4.379142761230469</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>8000</v>
       </c>
       <c r="B17" t="n">
-        <v>5.298005342483521</v>
+        <v>5.622652530670166</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>8500</v>
       </c>
       <c r="B18" t="n">
-        <v>6.243282794952393</v>
+        <v>6.23734450340271</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>9000</v>
       </c>
       <c r="B19" t="n">
-        <v>7.337611198425293</v>
+        <v>7.259650945663452</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>9500</v>
       </c>
       <c r="B20" t="n">
-        <v>8.386562585830688</v>
+        <v>8.340411424636841</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>10000</v>
       </c>
       <c r="B21" t="n">
-        <v>9.657172918319702</v>
+        <v>9.575966835021973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>